<commit_message>
Categorised AIF from SEBI in searching agent
</commit_message>
<xml_diff>
--- a/data/weekly_sebi_downloads.xlsx
+++ b/data/weekly_sebi_downloads.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Verticals</t>
   </si>
@@ -43,100 +43,76 @@
     <t>Path</t>
   </si>
   <si>
+    <t>AIF</t>
+  </si>
+  <si>
     <t>SEBI</t>
   </si>
   <si>
     <t>Circulars</t>
   </si>
   <si>
-    <t>Press Release</t>
-  </si>
-  <si>
     <t>Consulatation Paper</t>
   </si>
   <si>
     <t>2025</t>
   </si>
   <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>2025-11-25</t>
-  </si>
-  <si>
-    <t>2025-11-24</t>
-  </si>
-  <si>
-    <t>Specification of the terms and conditions for Debenture Trustees for carrying out activities outside the purview of SEBI</t>
-  </si>
-  <si>
-    <t>Modifications to Chapter IV of the Master Circular for Debenture Trustees dated August 13, 2025</t>
-  </si>
-  <si>
-    <t>Timeline for submission of information by the Issuer to the Debenture Trustee(s)</t>
-  </si>
-  <si>
-    <t>Memorandum of Understanding between Securities and Exchange Board of  India (SEBI) and National Forensic Sciences University (NFSU)</t>
-  </si>
-  <si>
-    <t>Ease of doing investment - Review of simplification of procedure and standardization of formats of documents for issuance of duplicate securities certificates.</t>
-  </si>
-  <si>
-    <t>Ease of investments and ease of doing business measures - Review of the Facility for Basic Services Demat Account (BSDA) for Financial Inclusion.</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/nov-2025/1764072855448.pdf</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/nov-2025/1764072737631.pdf</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/nov-2025/1764072664415.pdf</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/nov-2025/1764065882362.pdf</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/nov-2025/1764065506896.pdf</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/nov-2025/1763983154863.pdf</t>
-  </si>
-  <si>
-    <t>1764072855448.pdf</t>
-  </si>
-  <si>
-    <t>1764072737631.pdf</t>
-  </si>
-  <si>
-    <t>1764072664415.pdf</t>
-  </si>
-  <si>
-    <t>1764065882362.pdf</t>
-  </si>
-  <si>
-    <t>1764065506896.pdf</t>
-  </si>
-  <si>
-    <t>1763983154863.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Circulars/2025/November/1764072855448.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Circulars/2025/November/1764072737631.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Circulars/2025/November/1764072664415.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Press Release/2025/November/1764065882362.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Consulatation Paper/2025/November/1764065506896.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Consulatation Paper/2025/November/1763983154863.pdf</t>
+    <t>October</t>
+  </si>
+  <si>
+    <t>2025-10-24</t>
+  </si>
+  <si>
+    <t>2025-10-23</t>
+  </si>
+  <si>
+    <t>Transfer of portfolios of clients (PMS business) by Portfolio Managers.</t>
+  </si>
+  <si>
+    <t>Consultation paper for review of LODR Regulations - Clarification regarding the timeline for transfer of unclaimed amount by entity having listed non-convertible securities.</t>
+  </si>
+  <si>
+    <t>Circular on Relaxation of India geo-tagging for NRI clients re-KYCKYC modification through digital on-boarding video client Identification process (V-CIP)</t>
+  </si>
+  <si>
+    <t>Consultation paper on Standardization of process for Opening of Mutual Fund Folios and Execution of First Investment</t>
+  </si>
+  <si>
+    <t>https://www.sebi.gov.in/sebi_data/attachdocs/oct-2025/1761301360689.pdf</t>
+  </si>
+  <si>
+    <t>https://www.sebi.gov.in/sebi_data/attachdocs/oct-2025/1761306586026.pdf</t>
+  </si>
+  <si>
+    <t>https://www.sebi.gov.in/sebi_data/attachdocs/oct-2025/1761220376339.pdf</t>
+  </si>
+  <si>
+    <t>https://www.sebi.gov.in/sebi_data/attachdocs/oct-2025/1761210652019.pdf</t>
+  </si>
+  <si>
+    <t>1761301360689.pdf</t>
+  </si>
+  <si>
+    <t>1761306586026.pdf</t>
+  </si>
+  <si>
+    <t>1761220376339.pdf</t>
+  </si>
+  <si>
+    <t>1761210652019.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/AIF/Circulars/2025/October/1761301360689.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Consulatation Paper/2025/October/1761306586026.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Consulatation Paper/2025/October/1761220376339.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Consulatation Paper/2025/October/1761210652019.pdf</t>
   </si>
 </sst>
 </file>
@@ -507,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -547,7 +523,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -562,21 +538,21 @@
         <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
         <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -591,21 +567,21 @@
         <v>18</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
         <v>30</v>
-      </c>
-      <c r="I3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -614,27 +590,27 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
         <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -643,77 +619,19 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
         <v>32</v>
-      </c>
-      <c r="I5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -722,8 +640,6 @@
     <hyperlink ref="G3" r:id="rId2"/>
     <hyperlink ref="G4" r:id="rId3"/>
     <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tested again,but no changes in codebase
</commit_message>
<xml_diff>
--- a/data/weekly_sebi_downloads.xlsx
+++ b/data/weekly_sebi_downloads.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Verticals</t>
   </si>
@@ -46,109 +46,91 @@
     <t>Listed Companies</t>
   </si>
   <si>
-    <t>AIF</t>
-  </si>
-  <si>
     <t>SEBI</t>
   </si>
   <si>
-    <t>Circular-NSE</t>
-  </si>
-  <si>
     <t>Circular-BSE</t>
   </si>
   <si>
-    <t>Circulars</t>
+    <t>Press Release</t>
   </si>
   <si>
     <t>Consulatation Paper</t>
   </si>
   <si>
-    <t>Master circular</t>
-  </si>
-  <si>
     <t>2025</t>
   </si>
   <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>2025-10-14</t>
-  </si>
-  <si>
-    <t>2025-10-15</t>
-  </si>
-  <si>
-    <t>2025-10-13</t>
-  </si>
-  <si>
-    <t>2025-10-17</t>
-  </si>
-  <si>
-    <t>SEBI Circular on “Minimum information to be provided to the Audit Committee and Shareholders for approval of Related Party Transactions.”</t>
-  </si>
-  <si>
-    <t>Relaxation in timeline for disclosure of allocation methodology by Angel Funds</t>
-  </si>
-  <si>
-    <t>Minimum information to be provided to the Audit Committee and Shareholders for approval of Related Party Transactions</t>
-  </si>
-  <si>
-    <t>Consultation paper on proposed amendment to certain provisions of SEBI (LODR) Regulations, 2015 to facilitate transfer of securities transferred prior to April 1, 2019 and simplify the process of dematerialization of shares</t>
-  </si>
-  <si>
-    <t>Master Circular for issue and listing of Non-convertible Securities, Securitised Debt Instruments, Security Receipts, Municipal Debt Securities and Commercial Paper</t>
-  </si>
-  <si>
-    <t>https://nsearchives.nseindia.com//web/circular/2025-10/NSE_Circular_14102025_20251014172300.pdf</t>
-  </si>
-  <si>
-    <t>https://www.bseindia.com/markets/MarketInfo/DownloadAttach.aspx?id=20251014-34&amp;attachedId=dbe355c0-4b37-4967-8429-b7b6c97dbeba</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/oct-2025/1760525216783.pdf</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/oct-2025/1760356560260.pdf</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/oct-2025/1760699641194.pdf</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/oct-2025/1760532257519.pdf</t>
-  </si>
-  <si>
-    <t>SEBI_Circular_on_Minimum_information_to_be_provided_to_the_Audit_Committee_and_Shareholders_for_appr.pdf</t>
-  </si>
-  <si>
-    <t>1760525216783.pdf</t>
-  </si>
-  <si>
-    <t>1760356560260.pdf</t>
-  </si>
-  <si>
-    <t>1760699641194.pdf</t>
-  </si>
-  <si>
-    <t>1760532257519.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/Listed Companies/Circular-NSE/2025/October/SEBI_Circular_on_Minimum_information_to_be_provided_to_the_Audit_Committee_and_Shareholders_for_appr.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/Listed Companies/Circular-BSE/2025/October/SEBI_Circular_on_Minimum_information_to_be_provided_to_the_Audit_Committee_and_Shareholders_for_appr.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/AIF/Circulars/2025/October/1760525216783.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Circulars/2025/October/1760356560260.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Consulatation Paper/2025/October/1760699641194.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Master circular/2025/October/1760532257519.pdf</t>
+    <t>November</t>
+  </si>
+  <si>
+    <t>2025-11-21</t>
+  </si>
+  <si>
+    <t>2025-11-17</t>
+  </si>
+  <si>
+    <t>2025-11-19</t>
+  </si>
+  <si>
+    <t>Master Circular for issue and listing of Non-convertible Securities, Securitised Debt Instruments, Security Receipts, Municipal Debt Securities and Commercial Paper.</t>
+  </si>
+  <si>
+    <t>XBRL based filing of Regulation 50 for Entities which has listed its non-convertible securities</t>
+  </si>
+  <si>
+    <t>Frequently Asked Questions (FAQ) for submission of financial results as required under Regulation 33 of SEBI (LODR) Regulations, 2015 &amp; Master circular for compliance with the provisions of the SEBI (LODR) Regulations, 2015.</t>
+  </si>
+  <si>
+    <t>Caution to Public regarding unregistered Online Bond Platform Providers</t>
+  </si>
+  <si>
+    <t>Extension of timeline for submission of public comments on the consultation paper on 'Comprehensive review of SEBI (Mutual Funds) regulations, 1996'</t>
+  </si>
+  <si>
+    <t>https://www.bseindia.com/markets/MarketInfo/DownloadAttach.aspx?id=20251121-73&amp;attachedId=80bb176a-9beb-47e3-99ff-4832d65a2c1b</t>
+  </si>
+  <si>
+    <t>PrintToPDF</t>
+  </si>
+  <si>
+    <t>https://www.bseindia.com/markets/MarketInfo/DownloadAttach.aspx?id=20251117-20&amp;attachedId=7f776d85-62d5-4358-8d03-694f1de8f401</t>
+  </si>
+  <si>
+    <t>https://www.sebi.gov.in/sebi_data/attachdocs/nov-2025/1763551749033.pdf</t>
+  </si>
+  <si>
+    <t>https://www.sebi.gov.in/sebi_data/attachdocs/nov-2025/1763551731559.pdf</t>
+  </si>
+  <si>
+    <t>Master_Circular_for_issue_and_listing_of_Non_convertible_Securities_Securitised_Debt_Instruments_Sec.pdf</t>
+  </si>
+  <si>
+    <t>XBRL_based_filing_of_Regulation_50_for_Entities_which_has_listed_its_non_convertible_securities.pdf</t>
+  </si>
+  <si>
+    <t>Frequently_Asked_Questions_FAQ_for_submission_of_financial_results_as_required_under_Regulation_33_o.pdf</t>
+  </si>
+  <si>
+    <t>1763551749033.pdf</t>
+  </si>
+  <si>
+    <t>1763551731559.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/Listed Companies/Circular-BSE/2025/November/Master_Circular_for_issue_and_listing_of_Non_convertible_Securities_Securitised_Debt_Instruments_Sec.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/Listed Companies/Circular-BSE/2025/November/XBRL_based_filing_of_Regulation_50_for_Entities_which_has_listed_its_non_convertible_securities.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/Listed Companies/Circular-BSE/2025/November/Frequently_Asked_Questions_FAQ_for_submission_of_financial_results_as_required_under_Regulation_33_o.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Press Release/2025/November/1763551749033.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Consulatation Paper/2025/November/1763551731559.pdf</t>
   </si>
 </sst>
 </file>
@@ -519,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,28 +541,28 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
         <v>34</v>
-      </c>
-      <c r="I2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -588,154 +570,123 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" t="s">
         <v>38</v>
-      </c>
-      <c r="I7" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="G5" r:id="rId3"/>
+    <hyperlink ref="G6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed that BSE pdf URL issue
</commit_message>
<xml_diff>
--- a/data/weekly_sebi_downloads.xlsx
+++ b/data/weekly_sebi_downloads.xlsx
@@ -91,7 +91,7 @@
     <t>https://www.bseindia.com/markets/MarketInfo/DownloadAttach.aspx?id=20251121-73&amp;attachedId=80bb176a-9beb-47e3-99ff-4832d65a2c1b</t>
   </si>
   <si>
-    <t>PrintToPDF</t>
+    <t>https://www.bseindia.com/markets/MarketInfo/DispNewNoticesCirculars.aspx?page=20251121-72</t>
   </si>
   <si>
     <t>https://www.bseindia.com/markets/MarketInfo/DownloadAttach.aspx?id=20251117-20&amp;attachedId=7f776d85-62d5-4358-8d03-694f1de8f401</t>
@@ -584,7 +584,7 @@
       <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H3" t="s">
@@ -684,9 +684,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G4" r:id="rId2"/>
-    <hyperlink ref="G5" r:id="rId3"/>
-    <hyperlink ref="G6" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
AIF regulations prompt testing done
</commit_message>
<xml_diff>
--- a/data/weekly_sebi_downloads.xlsx
+++ b/data/weekly_sebi_downloads.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="tlEySi2KcqRk7bcKoJLueleZR+u1xtVhcQM9lXV9uDg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="8VG+5aypZWYbKqn7YeO1oc+ExJEz+m0pYkHEuEATax4="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Verticals</t>
   </si>
@@ -45,35 +45,38 @@
     <t>Path</t>
   </si>
   <si>
-    <t>SEBI</t>
-  </si>
-  <si>
-    <t>Circulars</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>2025-10-13</t>
-  </si>
-  <si>
-    <t>Minimum information to be provided to the Audit Committee and Shareholders for approval of Related Party Transactions</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/oct-2025/1760356560260.pdf</t>
-  </si>
-  <si>
-    <t>1760356560260.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Circulars/2025/October/1760356560260.pdf</t>
+    <t>AIF</t>
+  </si>
+  <si>
+    <t>Regulations</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>2025-12-11</t>
+  </si>
+  <si>
+    <t>Securities and Exchange Board of India (Real Estate Investment Trusts) Regulations, 2014  [Last amended on December 11, 2025]</t>
+  </si>
+  <si>
+    <t>https://www.sebi.gov.in/sebi_data/attachdocs/dec-2025/1765541474113.pdf</t>
+  </si>
+  <si>
+    <t>1765541474113.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs_test/Akshayam Data/AIF/Regulations/2025/December/1765541474113.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -87,8 +90,19 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11.0"/>
-      <color theme="1"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -120,19 +134,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -388,49 +399,58 @@
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3">
-        <v>2025.0</v>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
+        <v>17</v>
+      </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="3">
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9">
+      <c r="G9" s="4"/>
+    </row>
+    <row r="11">
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12">
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="G13" s="4"/>
+    </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -1407,10 +1427,17 @@
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="G2"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Consultation Paper and Master Circular
</commit_message>
<xml_diff>
--- a/data/weekly_sebi_downloads.xlsx
+++ b/data/weekly_sebi_downloads.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Verticals</t>
   </si>
@@ -46,43 +46,43 @@
     <t>SEBI</t>
   </si>
   <si>
-    <t>Press Release</t>
-  </si>
-  <si>
-    <t>2025</t>
+    <t>Master Circular</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>2025-09-23</t>
+  </si>
+  <si>
+    <t>Master Circular on Surveillance of Securities Market</t>
+  </si>
+  <si>
+    <t>https://www.sebi.gov.in/legal/master-circulars/sep-2024/master-circular-on-surveillance-of-securities-market_86929.html</t>
+  </si>
+  <si>
+    <t>1727094551693.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs_test/Akshayam Data/SEBI/Master Circular/2024/September/1727094551693.pdf</t>
   </si>
   <si>
     <t>December</t>
   </si>
   <si>
-    <t>2025-12-21</t>
-  </si>
-  <si>
-    <t>Clarification on a newsitem</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/dec-2025/1766319927198.pdf</t>
-  </si>
-  <si>
-    <t>1766319927198.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs_test/Akshayam Data/SEBI/Press Release/2025/December/1766319927198.pdf</t>
-  </si>
-  <si>
-    <t>2025-12-17</t>
-  </si>
-  <si>
-    <t>SEBI Board Meeting</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/dec-2025/1765977060104.pdf</t>
-  </si>
-  <si>
-    <t>1765977060104.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs_test/Akshayam Data/SEBI/Press Release/2025/December/1765977060104.pdf</t>
+    <t>2025-12-03</t>
+  </si>
+  <si>
+    <t>Master Circular for Depositories</t>
+  </si>
+  <si>
+    <t>https://www.sebi.gov.in/legal/master-circulars/dec-2024/master-circular-for-depositories_89245.html</t>
+  </si>
+  <si>
+    <t>1733233982158.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs_test/Akshayam Data/SEBI/Master Circular/2024/December/1733233982158.pdf</t>
   </si>
 </sst>
 </file>
@@ -90,7 +90,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +102,18 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -155,19 +167,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,15 +504,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="39.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -495,7 +522,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -518,60 +545,60 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4">
+        <v>2024</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="4">
+        <v>2024</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added MinIO for object storage
</commit_message>
<xml_diff>
--- a/data/weekly_sebi_downloads.xlsx
+++ b/data/weekly_sebi_downloads.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Verticals</t>
   </si>
@@ -46,43 +46,73 @@
     <t>SEBI</t>
   </si>
   <si>
-    <t>Press Release</t>
+    <t>Listed Companies</t>
+  </si>
+  <si>
+    <t>Circulars</t>
+  </si>
+  <si>
+    <t>Circular-BSE</t>
   </si>
   <si>
     <t>2025</t>
   </si>
   <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>2025-11-12</t>
-  </si>
-  <si>
-    <t>2025-11-10</t>
-  </si>
-  <si>
-    <t>Report of the High Level Committee on Conflict of Interest, Disclosures and  related matters in respect of Members and Officials of SEBI</t>
-  </si>
-  <si>
-    <t>High Level Committee on “Conflict of Interest, Disclosures and related matters in respect of Members and Officials of SEBI” submits its report</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/nov-2025/1762943978568.pdf</t>
-  </si>
-  <si>
-    <t>https://www.sebi.gov.in/sebi_data/attachdocs/nov-2025/1762786201875.pdf</t>
-  </si>
-  <si>
-    <t>1762943978568.pdf</t>
-  </si>
-  <si>
-    <t>1762786201875.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Press Release/2025/November/1762943978568.pdf</t>
-  </si>
-  <si>
-    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Press Release/2025/November/1762786201875.pdf</t>
+    <t>December</t>
+  </si>
+  <si>
+    <t>2025-12-24</t>
+  </si>
+  <si>
+    <t>2025-12-22</t>
+  </si>
+  <si>
+    <t>Ease of doing investment - Review of simplification of procedure and standardization of formats of documents for issuance of duplicate certificates</t>
+  </si>
+  <si>
+    <t>Ease of investments and ease of doing business measures – enhancing the ‘Facility for Basic Services Demat Account (BSDA)’</t>
+  </si>
+  <si>
+    <t>Modification in the conditions specified for reduction in denomination of debt securities</t>
+  </si>
+  <si>
+    <t>Mandating periodic disclosure requirements- Securitised Debt  Instruments (SDIs).</t>
+  </si>
+  <si>
+    <t>https://www.sebi.gov.in/sebi_data/attachdocs/dec-2025/1766582923860.pdf</t>
+  </si>
+  <si>
+    <t>https://www.sebi.gov.in/sebi_data/attachdocs/dec-2025/1766582690382.pdf</t>
+  </si>
+  <si>
+    <t>https://www.bseindia.com/markets/MarketInfo/DownloadAttach.aspx?id=20251222-26&amp;attachedId=0d20dbb4-212c-4f39-b26f-eb454f0b01f6</t>
+  </si>
+  <si>
+    <t>https://www.bseindia.com/markets/MarketInfo/DownloadAttach.aspx?id=20251222-25&amp;attachedId=346068c6-8cff-4f03-a397-067c6b16dff8</t>
+  </si>
+  <si>
+    <t>1766582923860.pdf</t>
+  </si>
+  <si>
+    <t>1766582690382.pdf</t>
+  </si>
+  <si>
+    <t>Modification_in_the_conditions_specified_for_reduction_in_denomination_of_debt_securities.pdf</t>
+  </si>
+  <si>
+    <t>Mandating_periodic_disclosure_requirements_Securitised_Debt_Instruments_SDIs.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Circulars/2025/December/1766582923860.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/SEBI/Circulars/2025/December/1766582690382.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/Listed Companies/Circular-BSE/2025/December/Modification_in_the_conditions_specified_for_reduction_in_denomination_of_debt_securities.pdf</t>
+  </si>
+  <si>
+    <t>/Users/admin/Downloads/Tejomaya_pdfs/Akshayam Data/Listed Companies/Circular-BSE/2025/December/Mandating_periodic_disclosure_requirements_Securitised_Debt_Instruments_SDIs.pdf</t>
   </si>
 </sst>
 </file>
@@ -453,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -493,28 +523,28 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -522,34 +552,94 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
-        <v>22</v>
+      <c r="G5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
     <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>